<commit_message>
added marine and future distributions
</commit_message>
<xml_diff>
--- a/data/renewables/Marine/tidal_lagoon_future_deployment_scenarios.xlsx
+++ b/data/renewables/Marine/tidal_lagoon_future_deployment_scenarios.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoe-my.sharepoint.com/personal/s1100626_ed_ac_uk/Documents/Year 2 - Energy System Modelling/Q3 - Analysis/Deployment scenarios/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoe-my.sharepoint.com/personal/alyden_ed_ac_uk/Documents/Python/PyPSA-GB v0.0.1/data/renewables/Marine/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_26B54EE290F6FF16DA66F7D3B5EE480360CA0FF7" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A82F5745-E974-4519-939A-57E511C60097}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12450"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tidal_lagoon_CT" sheetId="1" r:id="rId1"/>
@@ -80,9 +81,6 @@
     <t>Wat</t>
   </si>
   <si>
-    <t>S.W.Peninsula</t>
-  </si>
-  <si>
     <t>Blackpool</t>
   </si>
   <si>
@@ -102,12 +100,15 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>S.W.Penisula</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
@@ -425,20 +426,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <tabColor theme="7"/>
   </sheetPr>
   <dimension ref="A1:K21"/>
   <sheetViews>
-    <sheetView showZeros="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showZeros="0" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -473,12 +476,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
         <v>18</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
       </c>
       <c r="C2" s="2">
         <v>0</v>
@@ -505,10 +508,10 @@
         <v>-3.19</v>
       </c>
       <c r="K2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -543,7 +546,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -578,7 +581,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -613,12 +616,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
         <v>21</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
       </c>
       <c r="C6" s="2">
         <v>0</v>
@@ -645,10 +648,10 @@
         <v>-4.4000000000000004</v>
       </c>
       <c r="K6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -683,7 +686,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -715,12 +718,12 @@
         <v>-3.13</v>
       </c>
       <c r="K8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" s="2">
         <v>0</v>
@@ -743,51 +746,51 @@
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
     </row>
-    <row r="17" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
     </row>
-    <row r="18" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
     </row>
-    <row r="19" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
     </row>
-    <row r="20" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
     </row>
-    <row r="21" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -796,7 +799,7 @@
       <c r="H21" s="2"/>
     </row>
   </sheetData>
-  <sortState ref="A2:K8">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K8">
     <sortCondition ref="B2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -804,22 +807,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor rgb="FF00B0F0"/>
   </sheetPr>
   <dimension ref="A1:K21"/>
   <sheetViews>
     <sheetView showZeros="0" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -854,12 +857,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
         <v>18</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
       </c>
       <c r="C2" s="2">
         <v>0</v>
@@ -886,10 +889,10 @@
         <v>-3.19</v>
       </c>
       <c r="K2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -924,7 +927,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -959,7 +962,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -994,12 +997,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
         <v>21</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
       </c>
       <c r="C6" s="2">
         <v>0</v>
@@ -1026,10 +1029,10 @@
         <v>-4.4000000000000004</v>
       </c>
       <c r="K6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -1064,7 +1067,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -1096,12 +1099,12 @@
         <v>-3.13</v>
       </c>
       <c r="K8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" s="2">
         <v>0</v>
@@ -1124,51 +1127,51 @@
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
     </row>
-    <row r="17" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
     </row>
-    <row r="18" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
     </row>
-    <row r="19" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
     </row>
-    <row r="20" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
     </row>
-    <row r="21" spans="3:10" x14ac:dyDescent="0.35">
+    <row r="21" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -1177,7 +1180,7 @@
       <c r="H21" s="2"/>
     </row>
   </sheetData>
-  <sortState ref="A2:K8">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K8">
     <sortCondition ref="B2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1185,22 +1188,22 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView showZeros="0" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView showZeros="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1235,12 +1238,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
         <v>18</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
       </c>
       <c r="C2" s="2">
         <v>0</v>
@@ -1267,10 +1270,10 @@
         <v>-3.19</v>
       </c>
       <c r="K2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1305,7 +1308,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1340,7 +1343,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -1375,12 +1378,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
         <v>21</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
       </c>
       <c r="C6" s="2">
         <v>0</v>
@@ -1407,10 +1410,10 @@
         <v>-4.4000000000000004</v>
       </c>
       <c r="K6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -1445,7 +1448,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -1477,12 +1480,12 @@
         <v>-3.13</v>
       </c>
       <c r="K8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" s="2">
         <v>0</v>
@@ -1505,52 +1508,52 @@
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
     </row>
-    <row r="17" spans="9:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
     </row>
-    <row r="18" spans="9:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
     </row>
-    <row r="19" spans="9:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
     </row>
-    <row r="20" spans="9:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
     </row>
   </sheetData>
-  <sortState ref="A2:K8">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K8">
     <sortCondition ref="B2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1558,22 +1561,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <tabColor theme="6"/>
   </sheetPr>
   <dimension ref="A1:K20"/>
   <sheetViews>
     <sheetView showZeros="0" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1608,12 +1611,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
         <v>18</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
       </c>
       <c r="C2" s="2">
         <v>0</v>
@@ -1640,10 +1643,10 @@
         <v>-3.19</v>
       </c>
       <c r="K2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1678,7 +1681,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1713,7 +1716,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>13</v>
       </c>
@@ -1748,12 +1751,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
         <v>21</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
       </c>
       <c r="C6" s="2">
         <v>0</v>
@@ -1780,10 +1783,10 @@
         <v>-4.4000000000000004</v>
       </c>
       <c r="K6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>11</v>
       </c>
@@ -1818,7 +1821,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -1850,12 +1853,12 @@
         <v>-3.13</v>
       </c>
       <c r="K8" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9" s="2">
         <v>0</v>
@@ -1878,52 +1881,52 @@
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I10" s="3"/>
       <c r="J10" s="3"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
     </row>
-    <row r="17" spans="9:10" x14ac:dyDescent="0.35">
+    <row r="17" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I17" s="3"/>
       <c r="J17" s="3"/>
     </row>
-    <row r="18" spans="9:10" x14ac:dyDescent="0.35">
+    <row r="18" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I18" s="3"/>
       <c r="J18" s="3"/>
     </row>
-    <row r="19" spans="9:10" x14ac:dyDescent="0.35">
+    <row r="19" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I19" s="3"/>
       <c r="J19" s="3"/>
     </row>
-    <row r="20" spans="9:10" x14ac:dyDescent="0.35">
+    <row r="20" spans="9:10" x14ac:dyDescent="0.25">
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
     </row>
   </sheetData>
-  <sortState ref="A2:K8">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K8">
     <sortCondition ref="B2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1931,6 +1934,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010074D845749611EA4C8624BB0749477606" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="db22c31203cda416f2dbeab8713e41c9">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3e024f9b-2e2d-4f1c-b440-57efc902fc77" xmlns:ns4="5b3066ba-4cd6-475a-ab49-b036cbc58b74" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="d0a8c95347e59b8a6ed0a26052ccff3c" ns3:_="" ns4:_="">
     <xsd:import namespace="3e024f9b-2e2d-4f1c-b440-57efc902fc77"/>
@@ -2159,7 +2168,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -2168,13 +2177,24 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C9FFE97-E7CF-4434-9156-C8518CCA551B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="3e024f9b-2e2d-4f1c-b440-57efc902fc77"/>
+    <ds:schemaRef ds:uri="5b3066ba-4cd6-475a-ab49-b036cbc58b74"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C1FE2718-90D2-46FE-9A18-2807320E9FA6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2193,27 +2213,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4041BA3A-2CFE-4934-8B76-26286B1A928F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7C9FFE97-E7CF-4434-9156-C8518CCA551B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="3e024f9b-2e2d-4f1c-b440-57efc902fc77"/>
-    <ds:schemaRef ds:uri="5b3066ba-4cd6-475a-ab49-b036cbc58b74"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>